<commit_message>
Pipeline for HF case + dataset downloaded
</commit_message>
<xml_diff>
--- a/GridSearchCV_results/CKD_case/train_results_clf_fpipe_c.xlsx
+++ b/GridSearchCV_results/CKD_case/train_results_clf_fpipe_c.xlsx
@@ -786,16 +786,16 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.04786386489868164</v>
+        <v>0.04752969741821289</v>
       </c>
       <c r="C2">
-        <v>0.009958673706609932</v>
+        <v>0.01275396936339973</v>
       </c>
       <c r="D2">
-        <v>0.03231196403503418</v>
+        <v>0.02940793037414551</v>
       </c>
       <c r="E2">
-        <v>0.004397252801297821</v>
+        <v>0.006698448165590678</v>
       </c>
       <c r="F2" t="s">
         <v>63</v>
@@ -980,16 +980,16 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.05704360008239746</v>
+        <v>0.05816531181335449</v>
       </c>
       <c r="C3">
-        <v>0.003858632291855274</v>
+        <v>0.004787814655134202</v>
       </c>
       <c r="D3">
-        <v>0.03670015335083008</v>
+        <v>0.02771334648132324</v>
       </c>
       <c r="E3">
-        <v>0.004900991247301181</v>
+        <v>0.003613983533636935</v>
       </c>
       <c r="F3" t="s">
         <v>63</v>
@@ -1174,16 +1174,16 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.382166051864624</v>
+        <v>0.2795199871063233</v>
       </c>
       <c r="C4">
-        <v>0.02056884456193742</v>
+        <v>0.008223539453831995</v>
       </c>
       <c r="D4">
-        <v>0.05485234260559082</v>
+        <v>0.0405156135559082</v>
       </c>
       <c r="E4">
-        <v>0.008003190539803697</v>
+        <v>0.002483918768720574</v>
       </c>
       <c r="F4" t="s">
         <v>64</v>
@@ -1368,16 +1368,16 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.3368873119354248</v>
+        <v>0.2359130382537842</v>
       </c>
       <c r="C5">
-        <v>0.0723615356503214</v>
+        <v>0.04454885809408572</v>
       </c>
       <c r="D5">
-        <v>0.04328255653381348</v>
+        <v>0.0258641242980957</v>
       </c>
       <c r="E5">
-        <v>0.01060188390719646</v>
+        <v>0.006311647251569457</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>

</xml_diff>